<commit_message>
New 'TABC Summary Formatted' excel to replace the previous one
</commit_message>
<xml_diff>
--- a/app/public/csv/TABC Summary Formatted.xlsx
+++ b/app/public/csv/TABC Summary Formatted.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="TABC Inputs" sheetId="15" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2265" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2273" uniqueCount="79">
   <si>
     <t># existing telco buildings</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>C Route (routing to endpoints within 1/2 mile of B Route)</t>
+  </si>
+  <si>
+    <t>0 Employee</t>
   </si>
 </sst>
 </file>
@@ -912,7 +915,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1003"/>
+  <dimension ref="A1:G1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -922,13 +925,13 @@
     <col min="2" max="2" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>60</v>
       </c>
@@ -939,7 +942,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>74</v>
       </c>
@@ -949,8 +952,9 @@
       <c r="C4" s="37">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G4" s="28"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>74</v>
       </c>
@@ -960,8 +964,9 @@
       <c r="C5" s="37">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>74</v>
       </c>
@@ -972,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>74</v>
       </c>
@@ -983,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
         <v>74</v>
       </c>
@@ -994,7 +999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>74</v>
       </c>
@@ -1005,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
         <v>74</v>
       </c>
@@ -1016,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
         <v>74</v>
       </c>
@@ -1027,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="37" t="s">
         <v>74</v>
       </c>
@@ -1038,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
         <v>74</v>
       </c>
@@ -1049,7 +1054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>74</v>
       </c>
@@ -1060,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>74</v>
       </c>
@@ -1071,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>74</v>
       </c>
@@ -12099,7 +12104,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -12204,7 +12209,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="29">
-        <f>SUM(C53:G53)</f>
+        <f>SUM(D53:H53)</f>
         <v>0</v>
       </c>
     </row>
@@ -12441,7 +12446,7 @@
         <v>32</v>
       </c>
       <c r="C40" s="30">
-        <f>SUM(C45,C53:G53)</f>
+        <f>SUM(C45,D53:H53)</f>
         <v>0</v>
       </c>
     </row>
@@ -12507,27 +12512,30 @@
       <c r="H48" s="17"/>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="E49" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="25" t="s">
+      <c r="F49" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="25" t="s">
+      <c r="G49" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="25" t="s">
+      <c r="H49" s="25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="B50" s="13" t="s">
         <v>34</v>
@@ -12547,42 +12555,49 @@
       <c r="G50" s="29">
         <v>0</v>
       </c>
-      <c r="I50" s="33" t="s">
+      <c r="H50" s="29">
+        <v>0</v>
+      </c>
+      <c r="J50" s="33" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
+      <c r="C51" s="24"/>
       <c r="D51" s="13"/>
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
-      <c r="G51" s="17"/>
+      <c r="G51" s="13"/>
       <c r="H51" s="17"/>
       <c r="I51" s="17"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J51" s="17"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="E52" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="F52" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="G52" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="15" t="s">
+      <c r="H52" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
       <c r="B53" s="13" t="s">
         <v>33</v>
@@ -12602,7 +12617,10 @@
       <c r="G53" s="29">
         <v>0</v>
       </c>
-      <c r="I53" s="33" t="s">
+      <c r="H53" s="29">
+        <v>0</v>
+      </c>
+      <c r="J53" s="33" t="s">
         <v>67</v>
       </c>
     </row>
@@ -12614,9 +12632,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12719,7 +12739,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="29">
-        <f>SUM(C53:G53)</f>
+        <f>SUM(D53:H53)</f>
         <v>0</v>
       </c>
     </row>
@@ -12939,7 +12959,7 @@
         <v>32</v>
       </c>
       <c r="C40" s="30">
-        <f>SUM(C45,C53:G53)</f>
+        <f>SUM(C45,D53:H53)</f>
         <v>0</v>
       </c>
     </row>
@@ -13005,112 +13025,127 @@
       <c r="H48" s="26"/>
       <c r="I48" s="26"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="E49" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="25" t="s">
+      <c r="F49" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="25" t="s">
+      <c r="G49" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="25" t="s">
+      <c r="H49" s="25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="24"/>
       <c r="B50" s="24" t="s">
         <v>34</v>
       </c>
       <c r="C50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$I50&amp;" "&amp;C49,Calculations!$E$2:$E$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J50&amp;" "&amp;C49,Calculations!$E$2:$E$1001,1)</f>
         <v>0</v>
       </c>
       <c r="D50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$I50&amp;" "&amp;D49,Calculations!$E$2:$E$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J50&amp;" "&amp;D49,Calculations!$E$2:$E$1001,1)</f>
         <v>0</v>
       </c>
       <c r="E50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$I50&amp;" "&amp;E49,Calculations!$E$2:$E$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J50&amp;" "&amp;E49,Calculations!$E$2:$E$1001,1)</f>
         <v>0</v>
       </c>
       <c r="F50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$I50&amp;" "&amp;F49,Calculations!$E$2:$E$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J50&amp;" "&amp;F49,Calculations!$E$2:$E$1001,1)</f>
         <v>0</v>
       </c>
       <c r="G50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$I50&amp;" "&amp;G49,Calculations!$E$2:$E$1001,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I50" s="33" t="s">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J50&amp;" "&amp;G49,Calculations!$E$2:$E$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="29">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J50&amp;" "&amp;H49,Calculations!$E$2:$E$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J50" s="33" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="24"/>
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
       <c r="E51" s="24"/>
       <c r="F51" s="24"/>
-      <c r="G51" s="26"/>
+      <c r="G51" s="24"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J51" s="26"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C52" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="25" t="s">
+      <c r="E52" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="25" t="s">
+      <c r="F52" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F52" s="25" t="s">
+      <c r="G52" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="25" t="s">
+      <c r="H52" s="25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="24"/>
       <c r="B53" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$I53&amp;" "&amp;C52,Calculations!$E$2:$E$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J53&amp;" "&amp;C52,Calculations!$E$2:$E$1001,1)</f>
         <v>0</v>
       </c>
       <c r="D53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$I53&amp;" "&amp;D52,Calculations!$E$2:$E$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J53&amp;" "&amp;D52,Calculations!$E$2:$E$1001,1)</f>
         <v>0</v>
       </c>
       <c r="E53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$I53&amp;" "&amp;E52,Calculations!$E$2:$E$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J53&amp;" "&amp;E52,Calculations!$E$2:$E$1001,1)</f>
         <v>0</v>
       </c>
       <c r="F53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$I53&amp;" "&amp;F52,Calculations!$E$2:$E$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J53&amp;" "&amp;F52,Calculations!$E$2:$E$1001,1)</f>
         <v>0</v>
       </c>
       <c r="G53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$I53&amp;" "&amp;G52,Calculations!$E$2:$E$1001,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I53" s="33" t="s">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J53&amp;" "&amp;G52,Calculations!$E$2:$E$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="29">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'A Route Summary'!$J53&amp;" "&amp;H52,Calculations!$E$2:$E$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J53" s="33" t="s">
         <v>67</v>
       </c>
     </row>
@@ -13122,7 +13157,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -13227,7 +13262,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="29">
-        <f>SUM(C53:G53)</f>
+        <f>SUM(D53:H53)</f>
         <v>0</v>
       </c>
     </row>
@@ -13447,7 +13482,7 @@
         <v>32</v>
       </c>
       <c r="C40" s="30">
-        <f>SUM(C45,C53:G53)</f>
+        <f>SUM(C45,D53:H53)</f>
         <v>0</v>
       </c>
     </row>
@@ -13513,112 +13548,127 @@
       <c r="H48" s="26"/>
       <c r="I48" s="26"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="E49" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="25" t="s">
+      <c r="F49" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="25" t="s">
+      <c r="G49" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="25" t="s">
+      <c r="H49" s="25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="24"/>
       <c r="B50" s="24" t="s">
         <v>34</v>
       </c>
       <c r="C50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$I50&amp;" "&amp;C49,Calculations!$F$2:$F$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J50&amp;" "&amp;C49,Calculations!$F$2:$F$1001,1)</f>
         <v>0</v>
       </c>
       <c r="D50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$I50&amp;" "&amp;D49,Calculations!$F$2:$F$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J50&amp;" "&amp;D49,Calculations!$F$2:$F$1001,1)</f>
         <v>0</v>
       </c>
       <c r="E50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$I50&amp;" "&amp;E49,Calculations!$F$2:$F$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J50&amp;" "&amp;E49,Calculations!$F$2:$F$1001,1)</f>
         <v>0</v>
       </c>
       <c r="F50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$I50&amp;" "&amp;F49,Calculations!$F$2:$F$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J50&amp;" "&amp;F49,Calculations!$F$2:$F$1001,1)</f>
         <v>0</v>
       </c>
       <c r="G50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$I50&amp;" "&amp;G49,Calculations!$F$2:$F$1001,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I50" s="33" t="s">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J50&amp;" "&amp;G49,Calculations!$F$2:$F$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="29">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J50&amp;" "&amp;H49,Calculations!$F$2:$F$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J50" s="33" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="24"/>
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
       <c r="E51" s="24"/>
       <c r="F51" s="24"/>
-      <c r="G51" s="26"/>
+      <c r="G51" s="24"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J51" s="26"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C52" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="25" t="s">
+      <c r="E52" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="25" t="s">
+      <c r="F52" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F52" s="25" t="s">
+      <c r="G52" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="25" t="s">
+      <c r="H52" s="25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="24"/>
       <c r="B53" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$I53&amp;" "&amp;C52,Calculations!$F$2:$F$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J53&amp;" "&amp;C52,Calculations!$F$2:$F$1001,1)</f>
         <v>0</v>
       </c>
       <c r="D53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$I53&amp;" "&amp;D52,Calculations!$F$2:$F$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J53&amp;" "&amp;D52,Calculations!$F$2:$F$1001,1)</f>
         <v>0</v>
       </c>
       <c r="E53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$I53&amp;" "&amp;E52,Calculations!$F$2:$F$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J53&amp;" "&amp;E52,Calculations!$F$2:$F$1001,1)</f>
         <v>0</v>
       </c>
       <c r="F53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$I53&amp;" "&amp;F52,Calculations!$F$2:$F$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J53&amp;" "&amp;F52,Calculations!$F$2:$F$1001,1)</f>
         <v>0</v>
       </c>
       <c r="G53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$I53&amp;" "&amp;G52,Calculations!$F$2:$F$1001,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I53" s="33" t="s">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J53&amp;" "&amp;G52,Calculations!$F$2:$F$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="29">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$J53&amp;" "&amp;H52,Calculations!$F$2:$F$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J53" s="33" t="s">
         <v>67</v>
       </c>
     </row>
@@ -13630,11 +13680,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13737,7 +13785,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="29">
-        <f>SUM(C53:G53)</f>
+        <f>SUM(D53:H53)</f>
         <v>0</v>
       </c>
     </row>
@@ -13957,7 +14005,7 @@
         <v>32</v>
       </c>
       <c r="C40" s="30">
-        <f>SUM(C45,C53:G53)</f>
+        <f>SUM(C45,D53:H53)</f>
         <v>0</v>
       </c>
     </row>
@@ -14023,112 +14071,127 @@
       <c r="H48" s="26"/>
       <c r="I48" s="26"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="E49" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="25" t="s">
+      <c r="F49" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="25" t="s">
+      <c r="G49" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="25" t="s">
+      <c r="H49" s="25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="24"/>
       <c r="B50" s="24" t="s">
         <v>34</v>
       </c>
       <c r="C50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$I50&amp;" "&amp;C49,Calculations!$G$2:$G$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J50&amp;" "&amp;C49,Calculations!$G$2:$G$1001,1)</f>
         <v>0</v>
       </c>
       <c r="D50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$I50&amp;" "&amp;D49,Calculations!$G$2:$G$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J50&amp;" "&amp;D49,Calculations!$G$2:$G$1001,1)</f>
         <v>0</v>
       </c>
       <c r="E50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$I50&amp;" "&amp;E49,Calculations!$G$2:$G$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J50&amp;" "&amp;E49,Calculations!$G$2:$G$1001,1)</f>
         <v>0</v>
       </c>
       <c r="F50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$I50&amp;" "&amp;F49,Calculations!$G$2:$G$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J50&amp;" "&amp;F49,Calculations!$G$2:$G$1001,1)</f>
         <v>0</v>
       </c>
       <c r="G50" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$I50&amp;" "&amp;G49,Calculations!$G$2:$G$1001,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I50" s="33" t="s">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J50&amp;" "&amp;G49,Calculations!$G$2:$G$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="29">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J50&amp;" "&amp;H49,Calculations!$G$2:$G$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J50" s="33" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="24"/>
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
       <c r="E51" s="24"/>
       <c r="F51" s="24"/>
-      <c r="G51" s="26"/>
+      <c r="G51" s="24"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J51" s="26"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C52" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="25" t="s">
+      <c r="E52" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="25" t="s">
+      <c r="F52" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F52" s="25" t="s">
+      <c r="G52" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="25" t="s">
+      <c r="H52" s="25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="24"/>
       <c r="B53" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$I53&amp;" "&amp;C52,Calculations!$G$2:$G$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J53&amp;" "&amp;C52,Calculations!$G$2:$G$1001,1)</f>
         <v>0</v>
       </c>
       <c r="D53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$I53&amp;" "&amp;D52,Calculations!$G$2:$G$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J53&amp;" "&amp;D52,Calculations!$G$2:$G$1001,1)</f>
         <v>0</v>
       </c>
       <c r="E53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$I53&amp;" "&amp;E52,Calculations!$G$2:$G$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J53&amp;" "&amp;E52,Calculations!$G$2:$G$1001,1)</f>
         <v>0</v>
       </c>
       <c r="F53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$I53&amp;" "&amp;F52,Calculations!$G$2:$G$1001,1)</f>
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J53&amp;" "&amp;F52,Calculations!$G$2:$G$1001,1)</f>
         <v>0</v>
       </c>
       <c r="G53" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$I53&amp;" "&amp;G52,Calculations!$G$2:$G$1001,1)</f>
-        <v>0</v>
-      </c>
-      <c r="I53" s="33" t="s">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J53&amp;" "&amp;G52,Calculations!$G$2:$G$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="29">
+        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$J53&amp;" "&amp;H52,Calculations!$G$2:$G$1001,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J53" s="33" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
One more excel upload
</commit_message>
<xml_diff>
--- a/app/public/csv/TABC Summary Formatted.xlsx
+++ b/app/public/csv/TABC Summary Formatted.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -776,7 +776,7 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -847,6 +847,10 @@
     <xf numFmtId="5" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="01:  Hardcoded" xfId="4"/>
@@ -1641,7 +1645,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C16"/>
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,7 +1739,7 @@
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="46">
         <f>C46</f>
         <v>0</v>
       </c>
@@ -1744,7 +1748,7 @@
       <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="46">
         <f>SUM(C54:G54)</f>
         <v>0</v>
       </c>
@@ -2161,7 +2165,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C28"/>
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,8 +2260,8 @@
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$B11,Calculations!$E$2:$E$1001,1)</f>
+      <c r="C11" s="46">
+        <f>C46</f>
         <v>0</v>
       </c>
     </row>
@@ -2265,8 +2269,8 @@
       <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'B Route Summary'!$B12,Calculations!$E$2:$E$1001,1)</f>
+      <c r="C12" s="46">
+        <f>SUM(C54:G54)</f>
         <v>0</v>
       </c>
     </row>
@@ -2675,7 +2679,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2761,7 +2765,7 @@
       <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="46">
         <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$B10,Calculations!$F$2:$F$1001,1)</f>
         <v>0</v>
       </c>
@@ -2771,7 +2775,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$B11,Calculations!$F$2:$F$1001,1)</f>
+        <f>C46</f>
         <v>0</v>
       </c>
     </row>
@@ -2779,8 +2783,8 @@
       <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'C Route Summary'!$B12,Calculations!$F$2:$F$1001,1)</f>
+      <c r="C12" s="46">
+        <f>SUM(C54:G54)</f>
         <v>0</v>
       </c>
     </row>
@@ -3189,7 +3193,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3284,8 +3288,8 @@
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'D Route Summary'!$B11,Calculations!$G$2:$G$1001,1)</f>
+      <c r="C11" s="46">
+        <f>C46</f>
         <v>0</v>
       </c>
     </row>
@@ -3293,8 +3297,8 @@
       <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="29">
-        <f>SUMIFS(Calculations!$C$2:$C$1001,Calculations!$B$2:$B$1001,'D Route Summary'!$B12,Calculations!$G$2:$G$1001,1)</f>
+      <c r="C12" s="46">
+        <f>SUM(C54:G54)</f>
         <v>0</v>
       </c>
     </row>
@@ -3877,684 +3881,684 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="37">
+      <c r="A4" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="37">
+      <c r="A5" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="37">
+      <c r="A6" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="37">
+      <c r="A7" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="37">
+      <c r="A8" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="37">
+      <c r="A9" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="37">
+      <c r="A10" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="37">
+      <c r="A11" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="37">
+      <c r="A12" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="37">
+      <c r="A13" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="37">
+      <c r="A14" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="37">
+      <c r="A15" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="37">
+      <c r="A16" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="37">
+      <c r="A17" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="37">
+      <c r="A18" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="37">
+      <c r="A19" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="37">
+      <c r="A20" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="37">
+      <c r="A21" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="37">
+      <c r="A22" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="37">
+      <c r="A23" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="37">
+      <c r="A24" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="37">
+      <c r="A25" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="37">
+      <c r="A26" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="37">
+      <c r="A27" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="37">
+      <c r="A28" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="37">
+      <c r="A29" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="37">
+      <c r="A30" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="37">
+      <c r="A31" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="37">
+      <c r="A32" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="37">
+      <c r="A33" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="37">
+      <c r="A34" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="37">
+      <c r="A35" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="37">
+      <c r="A36" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="37">
+      <c r="A37" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="37">
+      <c r="A38" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="37">
+      <c r="A39" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="37">
+      <c r="A40" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="37">
+      <c r="A41" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="37">
+      <c r="A42" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="37">
+      <c r="A43" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="37">
+      <c r="A44" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C45" s="37">
+      <c r="A45" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="37">
+      <c r="A46" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" s="37">
+      <c r="A47" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="37">
+      <c r="A48" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" s="37">
+      <c r="A49" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="37">
+      <c r="A50" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B51" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C51" s="37">
+      <c r="A51" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="37">
+      <c r="A52" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B53" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="37">
+      <c r="A53" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B54" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="37">
+      <c r="A54" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B55" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="37">
+      <c r="A55" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C56" s="37">
+      <c r="A56" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B57" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="37">
+      <c r="A57" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B58" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C58" s="37">
+      <c r="A58" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B59" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C59" s="37">
+      <c r="A59" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C60" s="37">
+      <c r="A60" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B61" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" s="37">
+      <c r="A61" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B62" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C62" s="37">
+      <c r="A62" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B63" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" s="37">
+      <c r="A63" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B64" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C64" s="37">
+      <c r="A64" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="47">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B65" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C65" s="37">
+      <c r="A65" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="47">
         <v>0</v>
       </c>
     </row>

</xml_diff>